<commit_message>
by jiankong on 1113
</commit_message>
<xml_diff>
--- a/data/QC/质控组仪表盘10-2.xlsx
+++ b/data/QC/质控组仪表盘10-2.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>组别</t>
   </si>
@@ -86,9 +86,6 @@
     <t>48h通过率标线</t>
   </si>
   <si>
-    <t>质控组</t>
-  </si>
-  <si>
     <t>总体</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
   </si>
   <si>
     <t>下单错误数</t>
-  </si>
-  <si>
-    <t>张悦</t>
   </si>
   <si>
     <t>冷雪</t>
@@ -152,6 +146,9 @@
   <si>
     <t>10-2</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北京组</t>
   </si>
 </sst>
 </file>
@@ -508,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -531,102 +528,102 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>30</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>31</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>32</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>33</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>34</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>35</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>36</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>38</v>
-      </c>
-      <c r="R1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>191.82</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -634,46 +631,46 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D3">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>191.82</v>
+        <v>3.94</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>3.94</v>
       </c>
       <c r="I3">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="K3">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="N3">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="O3">
         <v>1</v>
@@ -682,65 +679,9 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>3.94</v>
-      </c>
-      <c r="H4">
-        <v>3.94</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>16</v>
-      </c>
-      <c r="N4">
-        <v>16</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
         <v>0</v>
       </c>
     </row>
@@ -755,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -834,13 +775,13 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D2">
         <v>29</v>
@@ -864,7 +805,7 @@
         <v>4.25</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>4.66</v>
       </c>
       <c r="L2">
         <v>26.49</v>

</xml_diff>